<commit_message>
Removed title on product.html and changed database location
</commit_message>
<xml_diff>
--- a/NeuroLINCS Milestones_10MAR2015_final.xlsx
+++ b/NeuroLINCS Milestones_10MAR2015_final.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="0" windowWidth="23100" windowHeight="13176" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1500" yWindow="0" windowWidth="23100" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HMS-Proposed Milestones Dec2014" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1106,7 +1111,7 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1121,7 +1126,7 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1136,10 +1141,10 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1148,16 +1153,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1169,7 +1174,7 @@
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color auto="1"/>
@@ -1185,7 +1190,7 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1196,7 +1201,7 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1209,7 +1214,7 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1226,7 +1231,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
@@ -1242,7 +1247,7 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1252,11 +1257,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1265,23 +1270,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1305,7 +1310,7 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
@@ -1317,28 +1322,28 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1352,13 +1357,13 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
@@ -1375,7 +1380,7 @@
         <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1388,7 +1393,7 @@
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1397,13 +1402,13 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1411,7 +1416,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="98">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1510,6 +1515,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1658,45 +1680,6 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="3" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1711,66 +1694,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="87" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="96" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="23" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="96" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1783,33 +1709,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="31" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="39" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="38" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1859,9 +1761,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="38" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1964,195 +1863,318 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="13" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="46" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="47" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="65" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="2" borderId="34" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="2" borderId="18" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="30" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="3" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="85" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="87" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="97" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="13" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="39" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="38" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="46" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="47" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="23" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="31" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="65" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="96" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="96" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="65" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="2" borderId="34" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="2" borderId="18" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="30" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="98">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2211,6 +2233,23 @@
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2586,55 +2625,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q177"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="54.3984375" customWidth="1"/>
+    <col min="1" max="2" width="54.375" customWidth="1"/>
     <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="35.09765625" customWidth="1"/>
-    <col min="10" max="10" width="19.3984375" customWidth="1"/>
+    <col min="9" max="9" width="35.125" customWidth="1"/>
+    <col min="10" max="10" width="19.375" customWidth="1"/>
     <col min="11" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="101.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="101.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="21">
       <c r="A3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76"/>
+    <row r="4" spans="1:13" ht="51" hidden="1" customHeight="1">
+      <c r="A4" s="188"/>
+      <c r="B4" s="188"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="8"/>
       <c r="I5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="21" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2644,11 +2683,11 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="66"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="200"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>6</v>
@@ -2665,7 +2704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="18">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
@@ -2688,11 +2727,11 @@
       <c r="L7" s="4"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.5" customHeight="1">
       <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="189" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -2719,9 +2758,9 @@
       </c>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="13"/>
-      <c r="B9" s="71"/>
+      <c r="B9" s="190"/>
       <c r="C9" s="12" t="s">
         <v>14</v>
       </c>
@@ -2746,9 +2785,9 @@
       </c>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" s="13"/>
-      <c r="B10" s="71"/>
+      <c r="B10" s="190"/>
       <c r="C10" s="12" t="s">
         <v>15</v>
       </c>
@@ -2773,9 +2812,9 @@
       </c>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="13"/>
-      <c r="B11" s="71"/>
+      <c r="B11" s="190"/>
       <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
@@ -2792,9 +2831,9 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="13"/>
-      <c r="B12" s="71"/>
+      <c r="B12" s="190"/>
       <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
@@ -2811,9 +2850,9 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="13"/>
-      <c r="B13" s="71"/>
+      <c r="B13" s="190"/>
       <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
@@ -2830,9 +2869,9 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="13"/>
-      <c r="B14" s="71"/>
+      <c r="B14" s="190"/>
       <c r="C14" s="12" t="s">
         <v>19</v>
       </c>
@@ -2847,9 +2886,9 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="13"/>
-      <c r="B15" s="71"/>
+      <c r="B15" s="190"/>
       <c r="C15" s="12" t="s">
         <v>20</v>
       </c>
@@ -2864,9 +2903,9 @@
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="13"/>
-      <c r="B16" s="71"/>
+      <c r="B16" s="190"/>
       <c r="C16" s="14" t="s">
         <v>22</v>
       </c>
@@ -2881,9 +2920,9 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="13"/>
-      <c r="B17" s="71"/>
+      <c r="B17" s="190"/>
       <c r="C17" s="14" t="s">
         <v>23</v>
       </c>
@@ -2898,9 +2937,9 @@
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="13"/>
-      <c r="B18" s="71"/>
+      <c r="B18" s="190"/>
       <c r="C18" s="14" t="s">
         <v>24</v>
       </c>
@@ -2915,9 +2954,9 @@
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="13"/>
-      <c r="B19" s="72"/>
+      <c r="B19" s="191"/>
       <c r="C19" s="14" t="s">
         <v>25</v>
       </c>
@@ -2932,7 +2971,7 @@
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="18">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
@@ -2955,11 +2994,11 @@
       <c r="L20" s="4"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15.5" customHeight="1">
       <c r="A21" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="189" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -2990,9 +3029,9 @@
       </c>
       <c r="M21" s="13"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="13"/>
-      <c r="B22" s="71"/>
+      <c r="B22" s="190"/>
       <c r="C22" s="12" t="s">
         <v>14</v>
       </c>
@@ -3019,9 +3058,9 @@
       </c>
       <c r="M22" s="13"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="13"/>
-      <c r="B23" s="71"/>
+      <c r="B23" s="190"/>
       <c r="C23" s="12" t="s">
         <v>15</v>
       </c>
@@ -3046,9 +3085,9 @@
       </c>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="13"/>
-      <c r="B24" s="71"/>
+      <c r="B24" s="190"/>
       <c r="C24" s="12" t="s">
         <v>16</v>
       </c>
@@ -3067,9 +3106,9 @@
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="13"/>
-      <c r="B25" s="71"/>
+      <c r="B25" s="190"/>
       <c r="C25" s="12" t="s">
         <v>17</v>
       </c>
@@ -3086,9 +3125,9 @@
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="13"/>
-      <c r="B26" s="71"/>
+      <c r="B26" s="190"/>
       <c r="C26" s="12" t="s">
         <v>18</v>
       </c>
@@ -3103,9 +3142,9 @@
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="13"/>
-      <c r="B27" s="71"/>
+      <c r="B27" s="190"/>
       <c r="C27" s="12" t="s">
         <v>19</v>
       </c>
@@ -3120,9 +3159,9 @@
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="13"/>
-      <c r="B28" s="71"/>
+      <c r="B28" s="190"/>
       <c r="C28" s="12" t="s">
         <v>20</v>
       </c>
@@ -3137,9 +3176,9 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="13"/>
-      <c r="B29" s="71"/>
+      <c r="B29" s="190"/>
       <c r="C29" s="14" t="s">
         <v>22</v>
       </c>
@@ -3154,9 +3193,9 @@
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="13"/>
-      <c r="B30" s="71"/>
+      <c r="B30" s="190"/>
       <c r="C30" s="14" t="s">
         <v>23</v>
       </c>
@@ -3171,9 +3210,9 @@
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="13"/>
-      <c r="B31" s="71"/>
+      <c r="B31" s="190"/>
       <c r="C31" s="14" t="s">
         <v>24</v>
       </c>
@@ -3188,9 +3227,9 @@
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="13"/>
-      <c r="B32" s="72"/>
+      <c r="B32" s="191"/>
       <c r="C32" s="14" t="s">
         <v>25</v>
       </c>
@@ -3205,7 +3244,7 @@
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
     </row>
-    <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="18">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
@@ -3228,11 +3267,11 @@
       <c r="L33" s="4"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="15.5" customHeight="1">
       <c r="A34" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="189" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -3263,9 +3302,9 @@
       </c>
       <c r="M34" s="13"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="13"/>
-      <c r="B35" s="71"/>
+      <c r="B35" s="190"/>
       <c r="C35" s="12" t="s">
         <v>14</v>
       </c>
@@ -3290,9 +3329,9 @@
       </c>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36" s="13"/>
-      <c r="B36" s="71"/>
+      <c r="B36" s="190"/>
       <c r="C36" s="12" t="s">
         <v>15</v>
       </c>
@@ -3317,9 +3356,9 @@
       </c>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13">
       <c r="A37" s="13"/>
-      <c r="B37" s="71"/>
+      <c r="B37" s="190"/>
       <c r="C37" s="12" t="s">
         <v>16</v>
       </c>
@@ -3344,9 +3383,9 @@
       </c>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13">
       <c r="A38" s="13"/>
-      <c r="B38" s="71"/>
+      <c r="B38" s="190"/>
       <c r="C38" s="12" t="s">
         <v>17</v>
       </c>
@@ -3363,9 +3402,9 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13">
       <c r="A39" s="13"/>
-      <c r="B39" s="71"/>
+      <c r="B39" s="190"/>
       <c r="C39" s="12" t="s">
         <v>18</v>
       </c>
@@ -3382,9 +3421,9 @@
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40" s="13"/>
-      <c r="B40" s="71"/>
+      <c r="B40" s="190"/>
       <c r="C40" s="12" t="s">
         <v>19</v>
       </c>
@@ -3401,9 +3440,9 @@
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13">
       <c r="A41" s="13"/>
-      <c r="B41" s="71"/>
+      <c r="B41" s="190"/>
       <c r="C41" s="12" t="s">
         <v>20</v>
       </c>
@@ -3418,9 +3457,9 @@
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="13"/>
-      <c r="B42" s="71"/>
+      <c r="B42" s="190"/>
       <c r="C42" s="14" t="s">
         <v>22</v>
       </c>
@@ -3435,9 +3474,9 @@
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43" s="13"/>
-      <c r="B43" s="71"/>
+      <c r="B43" s="190"/>
       <c r="C43" s="14" t="s">
         <v>23</v>
       </c>
@@ -3452,9 +3491,9 @@
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
       <c r="A44" s="13"/>
-      <c r="B44" s="71"/>
+      <c r="B44" s="190"/>
       <c r="C44" s="14" t="s">
         <v>24</v>
       </c>
@@ -3469,9 +3508,9 @@
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45" s="13"/>
-      <c r="B45" s="72"/>
+      <c r="B45" s="191"/>
       <c r="C45" s="14" t="s">
         <v>25</v>
       </c>
@@ -3486,14 +3525,14 @@
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
     </row>
-    <row r="46" spans="1:13" s="32" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" s="32" customFormat="1" ht="15.5" customHeight="1">
       <c r="A46" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="67" t="s">
+      <c r="B46" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="77" t="s">
+      <c r="C46" s="64" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="22"/>
@@ -3517,10 +3556,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" s="32" customFormat="1">
       <c r="A47" s="22"/>
-      <c r="B47" s="68"/>
-      <c r="C47" s="77" t="s">
+      <c r="B47" s="202"/>
+      <c r="C47" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="22"/>
@@ -3542,10 +3581,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" s="32" customFormat="1">
       <c r="A48" s="22"/>
-      <c r="B48" s="68"/>
-      <c r="C48" s="77" t="s">
+      <c r="B48" s="202"/>
+      <c r="C48" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="22"/>
@@ -3565,10 +3604,10 @@
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
     </row>
-    <row r="49" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" s="32" customFormat="1">
       <c r="A49" s="22"/>
-      <c r="B49" s="68"/>
-      <c r="C49" s="77" t="s">
+      <c r="B49" s="202"/>
+      <c r="C49" s="64" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="22"/>
@@ -3582,10 +3621,10 @@
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
     </row>
-    <row r="50" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" s="32" customFormat="1">
       <c r="A50" s="29"/>
-      <c r="B50" s="68"/>
-      <c r="C50" s="77" t="s">
+      <c r="B50" s="202"/>
+      <c r="C50" s="64" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="22"/>
@@ -3599,10 +3638,10 @@
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
     </row>
-    <row r="51" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" s="32" customFormat="1">
       <c r="A51" s="29"/>
-      <c r="B51" s="68"/>
-      <c r="C51" s="78" t="s">
+      <c r="B51" s="202"/>
+      <c r="C51" s="65" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="22"/>
@@ -3616,10 +3655,10 @@
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
     </row>
-    <row r="52" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" s="32" customFormat="1">
       <c r="A52" s="29"/>
-      <c r="B52" s="68"/>
-      <c r="C52" s="78" t="s">
+      <c r="B52" s="202"/>
+      <c r="C52" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="22"/>
@@ -3633,10 +3672,10 @@
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
-    <row r="53" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" s="32" customFormat="1">
       <c r="A53" s="29"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="78" t="s">
+      <c r="B53" s="203"/>
+      <c r="C53" s="65" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="22"/>
@@ -3650,14 +3689,14 @@
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
     </row>
-    <row r="54" spans="1:13" s="32" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" s="32" customFormat="1" ht="15.5" customHeight="1">
       <c r="A54" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C54" s="65" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="22"/>
@@ -3681,10 +3720,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" s="32" customFormat="1">
       <c r="A55" s="22"/>
-      <c r="B55" s="68"/>
-      <c r="C55" s="79" t="s">
+      <c r="B55" s="202"/>
+      <c r="C55" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="22"/>
@@ -3704,10 +3743,10 @@
       </c>
       <c r="M55" s="22"/>
     </row>
-    <row r="56" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" s="32" customFormat="1">
       <c r="A56" s="22"/>
-      <c r="B56" s="68"/>
-      <c r="C56" s="79" t="s">
+      <c r="B56" s="202"/>
+      <c r="C56" s="66" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="22"/>
@@ -3727,10 +3766,10 @@
       </c>
       <c r="M56" s="22"/>
     </row>
-    <row r="57" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" s="32" customFormat="1">
       <c r="A57" s="22"/>
-      <c r="B57" s="68"/>
-      <c r="C57" s="79" t="s">
+      <c r="B57" s="202"/>
+      <c r="C57" s="66" t="s">
         <v>25</v>
       </c>
       <c r="D57" s="22"/>
@@ -3744,9 +3783,9 @@
       <c r="L57" s="22"/>
       <c r="M57" s="22"/>
     </row>
-    <row r="58" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" s="32" customFormat="1">
       <c r="A58" s="29"/>
-      <c r="B58" s="68"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="33"/>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
@@ -3759,9 +3798,9 @@
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
     </row>
-    <row r="59" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" s="32" customFormat="1">
       <c r="A59" s="29"/>
-      <c r="B59" s="68"/>
+      <c r="B59" s="202"/>
       <c r="C59" s="33"/>
       <c r="D59" s="22"/>
       <c r="E59" s="22"/>
@@ -3774,9 +3813,9 @@
       <c r="L59" s="22"/>
       <c r="M59" s="22"/>
     </row>
-    <row r="60" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" s="32" customFormat="1">
       <c r="A60" s="29"/>
-      <c r="B60" s="68"/>
+      <c r="B60" s="202"/>
       <c r="C60" s="33"/>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
@@ -3789,9 +3828,9 @@
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
     </row>
-    <row r="61" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" s="32" customFormat="1">
       <c r="A61" s="29"/>
-      <c r="B61" s="68"/>
+      <c r="B61" s="202"/>
       <c r="C61" s="33"/>
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
@@ -3804,9 +3843,9 @@
       <c r="L61" s="22"/>
       <c r="M61" s="22"/>
     </row>
-    <row r="62" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" s="32" customFormat="1">
       <c r="A62" s="29"/>
-      <c r="B62" s="69"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="33"/>
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
@@ -3819,11 +3858,11 @@
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
     </row>
-    <row r="63" spans="1:13" s="32" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" s="32" customFormat="1" ht="15.5" customHeight="1">
       <c r="A63" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B63" s="67" t="s">
+      <c r="B63" s="201" t="s">
         <v>44</v>
       </c>
       <c r="C63" s="33"/>
@@ -3844,9 +3883,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" s="32" customFormat="1">
       <c r="A64" s="22"/>
-      <c r="B64" s="68"/>
+      <c r="B64" s="202"/>
       <c r="C64" s="33"/>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
@@ -3865,9 +3904,9 @@
       </c>
       <c r="M64" s="22"/>
     </row>
-    <row r="65" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" s="32" customFormat="1">
       <c r="A65" s="22"/>
-      <c r="B65" s="68"/>
+      <c r="B65" s="202"/>
       <c r="C65" s="33"/>
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
@@ -3884,9 +3923,9 @@
       </c>
       <c r="M65" s="22"/>
     </row>
-    <row r="66" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" s="32" customFormat="1">
       <c r="A66" s="22"/>
-      <c r="B66" s="68"/>
+      <c r="B66" s="202"/>
       <c r="C66" s="33"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
@@ -3899,9 +3938,9 @@
       <c r="L66" s="22"/>
       <c r="M66" s="22"/>
     </row>
-    <row r="67" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" s="32" customFormat="1">
       <c r="A67" s="29"/>
-      <c r="B67" s="68"/>
+      <c r="B67" s="202"/>
       <c r="C67" s="33"/>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
@@ -3914,9 +3953,9 @@
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
     </row>
-    <row r="68" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" s="32" customFormat="1">
       <c r="A68" s="29"/>
-      <c r="B68" s="68"/>
+      <c r="B68" s="202"/>
       <c r="C68" s="33"/>
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
@@ -3929,9 +3968,9 @@
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
     </row>
-    <row r="69" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" s="32" customFormat="1">
       <c r="A69" s="29"/>
-      <c r="B69" s="68"/>
+      <c r="B69" s="202"/>
       <c r="C69" s="33"/>
       <c r="D69" s="22"/>
       <c r="E69" s="22"/>
@@ -3944,9 +3983,9 @@
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
     </row>
-    <row r="70" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" s="32" customFormat="1">
       <c r="A70" s="29"/>
-      <c r="B70" s="68"/>
+      <c r="B70" s="202"/>
       <c r="C70" s="33"/>
       <c r="D70" s="22"/>
       <c r="E70" s="22"/>
@@ -3959,9 +3998,9 @@
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
     </row>
-    <row r="71" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" s="32" customFormat="1">
       <c r="A71" s="29"/>
-      <c r="B71" s="68"/>
+      <c r="B71" s="202"/>
       <c r="C71" s="33"/>
       <c r="D71" s="22"/>
       <c r="E71" s="22"/>
@@ -3974,9 +4013,9 @@
       <c r="L71" s="22"/>
       <c r="M71" s="22"/>
     </row>
-    <row r="72" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" s="32" customFormat="1">
       <c r="A72" s="29"/>
-      <c r="B72" s="68"/>
+      <c r="B72" s="202"/>
       <c r="C72" s="33"/>
       <c r="D72" s="22"/>
       <c r="E72" s="22"/>
@@ -3989,9 +4028,9 @@
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
     </row>
-    <row r="73" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" s="32" customFormat="1">
       <c r="A73" s="29"/>
-      <c r="B73" s="68"/>
+      <c r="B73" s="202"/>
       <c r="C73" s="33"/>
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
@@ -4004,9 +4043,9 @@
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
     </row>
-    <row r="74" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" s="32" customFormat="1">
       <c r="A74" s="29"/>
-      <c r="B74" s="69"/>
+      <c r="B74" s="203"/>
       <c r="C74" s="33"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
@@ -4019,17 +4058,17 @@
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
     </row>
-    <row r="75" spans="1:13" s="43" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="179" t="s">
+    <row r="75" spans="1:13" s="43" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A75" s="192" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="180" t="s">
+      <c r="B75" s="195" t="s">
         <v>135</v>
       </c>
       <c r="C75" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D75" s="181" t="s">
+      <c r="D75" s="137" t="s">
         <v>136</v>
       </c>
       <c r="E75" s="44"/>
@@ -4046,13 +4085,13 @@
         <v>21</v>
       </c>
       <c r="L75" s="39"/>
-      <c r="M75" s="182" t="s">
+      <c r="M75" s="138" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="183"/>
-      <c r="B76" s="184"/>
+    <row r="76" spans="1:13" s="43" customFormat="1">
+      <c r="A76" s="193"/>
+      <c r="B76" s="196"/>
       <c r="C76" s="16" t="s">
         <v>14</v>
       </c>
@@ -4061,7 +4100,7 @@
       <c r="F76" s="44"/>
       <c r="G76" s="44"/>
       <c r="H76" s="15"/>
-      <c r="I76" s="185" t="s">
+      <c r="I76" s="167" t="s">
         <v>139</v>
       </c>
       <c r="J76" s="15"/>
@@ -4069,9 +4108,9 @@
       <c r="L76" s="15"/>
       <c r="M76" s="15"/>
     </row>
-    <row r="77" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="186"/>
-      <c r="B77" s="184"/>
+    <row r="77" spans="1:13" s="43" customFormat="1">
+      <c r="A77" s="194"/>
+      <c r="B77" s="196"/>
       <c r="C77" s="16" t="s">
         <v>15</v>
       </c>
@@ -4080,15 +4119,15 @@
       <c r="F77" s="44"/>
       <c r="G77" s="44"/>
       <c r="H77" s="15"/>
-      <c r="I77" s="187"/>
+      <c r="I77" s="168"/>
       <c r="J77" s="15"/>
       <c r="K77" s="15"/>
       <c r="L77" s="15"/>
       <c r="M77" s="15"/>
     </row>
-    <row r="78" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" s="43" customFormat="1">
       <c r="A78" s="44"/>
-      <c r="B78" s="184"/>
+      <c r="B78" s="196"/>
       <c r="C78" s="16" t="s">
         <v>16</v>
       </c>
@@ -4097,15 +4136,15 @@
       <c r="F78" s="44"/>
       <c r="G78" s="44"/>
       <c r="H78" s="15"/>
-      <c r="I78" s="188"/>
+      <c r="I78" s="169"/>
       <c r="J78" s="15"/>
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
-      <c r="M78" s="182"/>
-    </row>
-    <row r="79" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M78" s="138"/>
+    </row>
+    <row r="79" spans="1:13" s="43" customFormat="1">
       <c r="A79" s="44"/>
-      <c r="B79" s="184"/>
+      <c r="B79" s="196"/>
       <c r="C79" s="16" t="s">
         <v>17</v>
       </c>
@@ -4120,9 +4159,9 @@
       <c r="L79" s="15"/>
       <c r="M79" s="15"/>
     </row>
-    <row r="80" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" s="43" customFormat="1">
       <c r="A80" s="44"/>
-      <c r="B80" s="189"/>
+      <c r="B80" s="139"/>
       <c r="C80" s="17" t="s">
         <v>18</v>
       </c>
@@ -4137,9 +4176,9 @@
       <c r="L80" s="15"/>
       <c r="M80" s="15"/>
     </row>
-    <row r="81" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" s="43" customFormat="1">
       <c r="A81" s="44"/>
-      <c r="B81" s="189"/>
+      <c r="B81" s="139"/>
       <c r="C81" s="17" t="s">
         <v>19</v>
       </c>
@@ -4154,9 +4193,9 @@
       <c r="L81" s="15"/>
       <c r="M81" s="15"/>
     </row>
-    <row r="82" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" s="43" customFormat="1">
       <c r="A82" s="44"/>
-      <c r="B82" s="189"/>
+      <c r="B82" s="139"/>
       <c r="C82" s="17" t="s">
         <v>20</v>
       </c>
@@ -4171,9 +4210,9 @@
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
     </row>
-    <row r="83" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" s="43" customFormat="1">
       <c r="A83" s="44"/>
-      <c r="B83" s="189"/>
+      <c r="B83" s="139"/>
       <c r="C83" s="17" t="s">
         <v>22</v>
       </c>
@@ -4188,10 +4227,10 @@
       <c r="L83" s="15"/>
       <c r="M83" s="15"/>
     </row>
-    <row r="84" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" s="43" customFormat="1">
       <c r="A84" s="44"/>
-      <c r="B84" s="189"/>
-      <c r="C84" s="190" t="s">
+      <c r="B84" s="139"/>
+      <c r="C84" s="140" t="s">
         <v>23</v>
       </c>
       <c r="D84" s="44"/>
@@ -4205,10 +4244,10 @@
       <c r="L84" s="15"/>
       <c r="M84" s="15"/>
     </row>
-    <row r="85" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" s="43" customFormat="1">
       <c r="A85" s="44"/>
-      <c r="B85" s="189"/>
-      <c r="C85" s="190" t="s">
+      <c r="B85" s="139"/>
+      <c r="C85" s="140" t="s">
         <v>24</v>
       </c>
       <c r="D85" s="44"/>
@@ -4222,10 +4261,10 @@
       <c r="L85" s="15"/>
       <c r="M85" s="15"/>
     </row>
-    <row r="86" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" s="43" customFormat="1">
       <c r="A86" s="44"/>
-      <c r="B86" s="189"/>
-      <c r="C86" s="190" t="s">
+      <c r="B86" s="139"/>
+      <c r="C86" s="140" t="s">
         <v>25</v>
       </c>
       <c r="D86" s="44"/>
@@ -4239,11 +4278,11 @@
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
     </row>
-    <row r="87" spans="1:13" s="43" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="191" t="s">
+    <row r="87" spans="1:13" s="43" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A87" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="B87" s="192" t="s">
+      <c r="B87" s="173" t="s">
         <v>141</v>
       </c>
       <c r="C87" s="20" t="s">
@@ -4256,19 +4295,19 @@
       <c r="F87" s="19"/>
       <c r="G87" s="19"/>
       <c r="H87" s="19"/>
-      <c r="I87" s="193" t="s">
+      <c r="I87" s="141" t="s">
         <v>137</v>
       </c>
       <c r="J87" s="19"/>
       <c r="K87" s="19"/>
       <c r="L87" s="19"/>
-      <c r="M87" s="194" t="s">
+      <c r="M87" s="142" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="195"/>
-      <c r="B88" s="196"/>
+    <row r="88" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A88" s="171"/>
+      <c r="B88" s="174"/>
       <c r="C88" s="20" t="s">
         <v>14</v>
       </c>
@@ -4279,17 +4318,17 @@
       <c r="F88" s="40"/>
       <c r="G88" s="40"/>
       <c r="H88" s="40"/>
-      <c r="I88" s="197" t="s">
+      <c r="I88" s="176" t="s">
         <v>139</v>
       </c>
       <c r="J88" s="40"/>
       <c r="K88" s="40"/>
       <c r="L88" s="40"/>
-      <c r="M88" s="198"/>
-    </row>
-    <row r="89" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="199"/>
-      <c r="B89" s="200"/>
+      <c r="M88" s="143"/>
+    </row>
+    <row r="89" spans="1:13" s="43" customFormat="1">
+      <c r="A89" s="172"/>
+      <c r="B89" s="175"/>
       <c r="C89" s="20" t="s">
         <v>15</v>
       </c>
@@ -4298,15 +4337,15 @@
       <c r="F89" s="40"/>
       <c r="G89" s="40"/>
       <c r="H89" s="40"/>
-      <c r="I89" s="201"/>
+      <c r="I89" s="177"/>
       <c r="J89" s="40"/>
       <c r="K89" s="40"/>
       <c r="L89" s="40"/>
-      <c r="M89" s="198"/>
-    </row>
-    <row r="90" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M89" s="143"/>
+    </row>
+    <row r="90" spans="1:13" s="43" customFormat="1">
       <c r="A90" s="40"/>
-      <c r="B90" s="202" t="s">
+      <c r="B90" s="144" t="s">
         <v>144</v>
       </c>
       <c r="C90" s="20" t="s">
@@ -4317,7 +4356,7 @@
       <c r="F90" s="40"/>
       <c r="G90" s="40"/>
       <c r="H90" s="40"/>
-      <c r="I90" s="203"/>
+      <c r="I90" s="178"/>
       <c r="J90" s="40" t="s">
         <v>10</v>
       </c>
@@ -4325,11 +4364,11 @@
         <v>21</v>
       </c>
       <c r="L90" s="40"/>
-      <c r="M90" s="198"/>
-    </row>
-    <row r="91" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M90" s="143"/>
+    </row>
+    <row r="91" spans="1:13" s="43" customFormat="1">
       <c r="A91" s="40"/>
-      <c r="B91" s="204" t="s">
+      <c r="B91" s="145" t="s">
         <v>29</v>
       </c>
       <c r="C91" s="20" t="s">
@@ -4346,11 +4385,11 @@
         <v>93</v>
       </c>
       <c r="L91" s="40"/>
-      <c r="M91" s="198"/>
-    </row>
-    <row r="92" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M91" s="143"/>
+    </row>
+    <row r="92" spans="1:13" s="43" customFormat="1">
       <c r="A92" s="40"/>
-      <c r="B92" s="204" t="s">
+      <c r="B92" s="145" t="s">
         <v>30</v>
       </c>
       <c r="C92" s="21" t="s">
@@ -4367,11 +4406,11 @@
         <v>93</v>
       </c>
       <c r="L92" s="40"/>
-      <c r="M92" s="198"/>
-    </row>
-    <row r="93" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M92" s="143"/>
+    </row>
+    <row r="93" spans="1:13" s="43" customFormat="1">
       <c r="A93" s="40"/>
-      <c r="B93" s="204"/>
+      <c r="B93" s="145"/>
       <c r="C93" s="21" t="s">
         <v>19</v>
       </c>
@@ -4384,9 +4423,9 @@
       <c r="J93" s="40"/>
       <c r="K93" s="40"/>
       <c r="L93" s="40"/>
-      <c r="M93" s="198"/>
-    </row>
-    <row r="94" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M93" s="143"/>
+    </row>
+    <row r="94" spans="1:13" s="43" customFormat="1">
       <c r="A94" s="40"/>
       <c r="B94" s="18"/>
       <c r="C94" s="21" t="s">
@@ -4401,11 +4440,11 @@
       <c r="J94" s="40"/>
       <c r="K94" s="40"/>
       <c r="L94" s="40"/>
-      <c r="M94" s="198"/>
-    </row>
-    <row r="95" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M94" s="143"/>
+    </row>
+    <row r="95" spans="1:13" s="43" customFormat="1">
       <c r="A95" s="40"/>
-      <c r="B95" s="204"/>
+      <c r="B95" s="145"/>
       <c r="C95" s="21" t="s">
         <v>22</v>
       </c>
@@ -4418,12 +4457,12 @@
       <c r="J95" s="40"/>
       <c r="K95" s="40"/>
       <c r="L95" s="40"/>
-      <c r="M95" s="198"/>
-    </row>
-    <row r="96" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M95" s="143"/>
+    </row>
+    <row r="96" spans="1:13" s="43" customFormat="1">
       <c r="A96" s="40"/>
       <c r="B96" s="18"/>
-      <c r="C96" s="205" t="s">
+      <c r="C96" s="146" t="s">
         <v>23</v>
       </c>
       <c r="D96" s="18"/>
@@ -4437,10 +4476,10 @@
       <c r="L96" s="40"/>
       <c r="M96" s="40"/>
     </row>
-    <row r="97" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" s="43" customFormat="1">
       <c r="A97" s="40"/>
       <c r="B97" s="18"/>
-      <c r="C97" s="205" t="s">
+      <c r="C97" s="146" t="s">
         <v>24</v>
       </c>
       <c r="D97" s="18"/>
@@ -4454,10 +4493,10 @@
       <c r="L97" s="40"/>
       <c r="M97" s="40"/>
     </row>
-    <row r="98" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" s="43" customFormat="1">
       <c r="A98" s="40"/>
-      <c r="B98" s="204"/>
-      <c r="C98" s="205" t="s">
+      <c r="B98" s="145"/>
+      <c r="C98" s="146" t="s">
         <v>25</v>
       </c>
       <c r="D98" s="18"/>
@@ -4471,14 +4510,14 @@
       <c r="L98" s="40"/>
       <c r="M98" s="40"/>
     </row>
-    <row r="99" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="206" t="s">
+    <row r="99" spans="1:13" s="8" customFormat="1">
+      <c r="A99" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="B99" s="207" t="s">
+      <c r="B99" s="179" t="s">
         <v>145</v>
       </c>
-      <c r="C99" s="208" t="s">
+      <c r="C99" s="148" t="s">
         <v>13</v>
       </c>
       <c r="D99" s="23" t="s">
@@ -4488,20 +4527,20 @@
       <c r="F99" s="41"/>
       <c r="G99" s="41"/>
       <c r="H99" s="41"/>
-      <c r="I99" s="209" t="s">
+      <c r="I99" s="149" t="s">
         <v>137</v>
       </c>
       <c r="J99" s="41"/>
       <c r="K99" s="41"/>
       <c r="L99" s="41"/>
-      <c r="M99" s="210" t="s">
+      <c r="M99" s="150" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A100" s="41"/>
-      <c r="B100" s="211"/>
-      <c r="C100" s="212" t="s">
+      <c r="B100" s="180"/>
+      <c r="C100" s="151" t="s">
         <v>14</v>
       </c>
       <c r="D100" s="23" t="s">
@@ -4511,7 +4550,7 @@
       <c r="F100" s="41"/>
       <c r="G100" s="41"/>
       <c r="H100" s="41"/>
-      <c r="I100" s="213" t="s">
+      <c r="I100" s="182" t="s">
         <v>146</v>
       </c>
       <c r="J100" s="41"/>
@@ -4519,10 +4558,10 @@
       <c r="L100" s="41"/>
       <c r="M100" s="41"/>
     </row>
-    <row r="101" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" s="43" customFormat="1">
       <c r="A101" s="41"/>
-      <c r="B101" s="214"/>
-      <c r="C101" s="212" t="s">
+      <c r="B101" s="181"/>
+      <c r="C101" s="151" t="s">
         <v>15</v>
       </c>
       <c r="D101" s="23"/>
@@ -4530,18 +4569,18 @@
       <c r="F101" s="41"/>
       <c r="G101" s="41"/>
       <c r="H101" s="41"/>
-      <c r="I101" s="215"/>
+      <c r="I101" s="183"/>
       <c r="J101" s="41"/>
       <c r="K101" s="41"/>
       <c r="L101" s="41"/>
       <c r="M101" s="41"/>
     </row>
-    <row r="102" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" s="43" customFormat="1">
       <c r="A102" s="41"/>
       <c r="B102" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C102" s="212" t="s">
+      <c r="C102" s="151" t="s">
         <v>16</v>
       </c>
       <c r="D102" s="23"/>
@@ -4549,7 +4588,7 @@
       <c r="F102" s="41"/>
       <c r="G102" s="41"/>
       <c r="H102" s="41"/>
-      <c r="I102" s="216"/>
+      <c r="I102" s="184"/>
       <c r="J102" s="41"/>
       <c r="K102" s="41" t="s">
         <v>93</v>
@@ -4559,12 +4598,12 @@
       </c>
       <c r="M102" s="41"/>
     </row>
-    <row r="103" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" s="43" customFormat="1">
       <c r="A103" s="41"/>
       <c r="B103" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C103" s="212" t="s">
+      <c r="C103" s="151" t="s">
         <v>17</v>
       </c>
       <c r="D103" s="23"/>
@@ -4582,12 +4621,12 @@
       </c>
       <c r="M103" s="41"/>
     </row>
-    <row r="104" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" s="43" customFormat="1">
       <c r="A104" s="41"/>
       <c r="B104" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C104" s="212" t="s">
+      <c r="C104" s="151" t="s">
         <v>18</v>
       </c>
       <c r="D104" s="23"/>
@@ -4605,10 +4644,10 @@
       </c>
       <c r="M104" s="41"/>
     </row>
-    <row r="105" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" s="43" customFormat="1">
       <c r="A105" s="41"/>
       <c r="B105" s="41"/>
-      <c r="C105" s="212" t="s">
+      <c r="C105" s="151" t="s">
         <v>19</v>
       </c>
       <c r="D105" s="23"/>
@@ -4622,10 +4661,10 @@
       <c r="L105" s="41"/>
       <c r="M105" s="41"/>
     </row>
-    <row r="106" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" s="43" customFormat="1">
       <c r="A106" s="41"/>
       <c r="B106" s="41"/>
-      <c r="C106" s="212" t="s">
+      <c r="C106" s="151" t="s">
         <v>20</v>
       </c>
       <c r="D106" s="23"/>
@@ -4639,10 +4678,10 @@
       <c r="L106" s="41"/>
       <c r="M106" s="41"/>
     </row>
-    <row r="107" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" s="43" customFormat="1">
       <c r="A107" s="41"/>
       <c r="B107" s="41"/>
-      <c r="C107" s="212" t="s">
+      <c r="C107" s="151" t="s">
         <v>22</v>
       </c>
       <c r="D107" s="23"/>
@@ -4656,10 +4695,10 @@
       <c r="L107" s="41"/>
       <c r="M107" s="41"/>
     </row>
-    <row r="108" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" s="43" customFormat="1">
       <c r="A108" s="41"/>
       <c r="B108" s="41"/>
-      <c r="C108" s="212" t="s">
+      <c r="C108" s="151" t="s">
         <v>23</v>
       </c>
       <c r="D108" s="23"/>
@@ -4673,7 +4712,7 @@
       <c r="L108" s="41"/>
       <c r="M108" s="41"/>
     </row>
-    <row r="109" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" s="43" customFormat="1">
       <c r="A109" s="41"/>
       <c r="B109" s="41"/>
       <c r="C109" s="24" t="s">
@@ -4690,7 +4729,7 @@
       <c r="L109" s="41"/>
       <c r="M109" s="41"/>
     </row>
-    <row r="110" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" s="43" customFormat="1">
       <c r="A110" s="41"/>
       <c r="B110" s="41"/>
       <c r="C110" s="24" t="s">
@@ -4707,11 +4746,11 @@
       <c r="L110" s="41"/>
       <c r="M110" s="41"/>
     </row>
-    <row r="111" spans="1:13" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A111" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B111" s="217" t="s">
+      <c r="B111" s="163" t="s">
         <v>147</v>
       </c>
       <c r="C111" s="25" t="s">
@@ -4724,19 +4763,19 @@
       <c r="F111" s="42"/>
       <c r="G111" s="42"/>
       <c r="H111" s="42"/>
-      <c r="I111" s="218" t="s">
+      <c r="I111" s="152" t="s">
         <v>137</v>
       </c>
       <c r="J111" s="42"/>
       <c r="K111" s="42"/>
       <c r="L111" s="42"/>
-      <c r="M111" s="219" t="s">
+      <c r="M111" s="153" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A112" s="42"/>
-      <c r="B112" s="220"/>
+      <c r="B112" s="164"/>
       <c r="C112" s="25" t="s">
         <v>14</v>
       </c>
@@ -4747,7 +4786,7 @@
       <c r="F112" s="42"/>
       <c r="G112" s="42"/>
       <c r="H112" s="42"/>
-      <c r="I112" s="221" t="s">
+      <c r="I112" s="160" t="s">
         <v>139</v>
       </c>
       <c r="J112" s="42"/>
@@ -4755,9 +4794,9 @@
       <c r="L112" s="42"/>
       <c r="M112" s="42"/>
     </row>
-    <row r="113" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A113" s="42"/>
-      <c r="B113" s="222"/>
+      <c r="B113" s="197"/>
       <c r="C113" s="25" t="s">
         <v>15</v>
       </c>
@@ -4766,13 +4805,13 @@
       <c r="F113" s="42"/>
       <c r="G113" s="42"/>
       <c r="H113" s="42"/>
-      <c r="I113" s="223"/>
+      <c r="I113" s="161"/>
       <c r="J113" s="42"/>
       <c r="K113" s="42"/>
       <c r="L113" s="42"/>
       <c r="M113" s="42"/>
     </row>
-    <row r="114" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A114" s="42"/>
       <c r="B114" s="42" t="s">
         <v>148</v>
@@ -4785,7 +4824,7 @@
       <c r="F114" s="42"/>
       <c r="G114" s="42"/>
       <c r="H114" s="42"/>
-      <c r="I114" s="224"/>
+      <c r="I114" s="162"/>
       <c r="J114" s="42"/>
       <c r="K114" s="42"/>
       <c r="L114" s="42" t="s">
@@ -4793,9 +4832,9 @@
       </c>
       <c r="M114" s="42"/>
     </row>
-    <row r="115" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A115" s="42"/>
-      <c r="B115" s="217" t="s">
+      <c r="B115" s="163" t="s">
         <v>149</v>
       </c>
       <c r="C115" s="27" t="s">
@@ -4806,7 +4845,7 @@
       <c r="F115" s="42"/>
       <c r="G115" s="42"/>
       <c r="H115" s="42"/>
-      <c r="I115" s="221" t="s">
+      <c r="I115" s="160" t="s">
         <v>146</v>
       </c>
       <c r="J115" s="42"/>
@@ -4816,9 +4855,9 @@
       </c>
       <c r="M115" s="42"/>
     </row>
-    <row r="116" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A116" s="42"/>
-      <c r="B116" s="220"/>
+      <c r="B116" s="164"/>
       <c r="C116" s="27" t="s">
         <v>18</v>
       </c>
@@ -4827,15 +4866,15 @@
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
       <c r="H116" s="42"/>
-      <c r="I116" s="223"/>
+      <c r="I116" s="161"/>
       <c r="J116" s="42"/>
       <c r="K116" s="42"/>
       <c r="L116" s="42"/>
       <c r="M116" s="42"/>
     </row>
-    <row r="117" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A117" s="42"/>
-      <c r="B117" s="225" t="s">
+      <c r="B117" s="154" t="s">
         <v>150</v>
       </c>
       <c r="C117" s="27" t="s">
@@ -4846,7 +4885,7 @@
       <c r="F117" s="42"/>
       <c r="G117" s="42"/>
       <c r="H117" s="42"/>
-      <c r="I117" s="223"/>
+      <c r="I117" s="161"/>
       <c r="J117" s="42"/>
       <c r="K117" s="42"/>
       <c r="L117" s="42" t="s">
@@ -4854,9 +4893,9 @@
       </c>
       <c r="M117" s="42"/>
     </row>
-    <row r="118" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" s="43" customFormat="1">
       <c r="A118" s="42"/>
-      <c r="B118" s="226" t="s">
+      <c r="B118" s="165" t="s">
         <v>151</v>
       </c>
       <c r="C118" s="27" t="s">
@@ -4875,9 +4914,9 @@
       </c>
       <c r="M118" s="42"/>
     </row>
-    <row r="119" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" s="43" customFormat="1" ht="15.75" customHeight="1">
       <c r="A119" s="42"/>
-      <c r="B119" s="227"/>
+      <c r="B119" s="166"/>
       <c r="C119" s="27" t="s">
         <v>22</v>
       </c>
@@ -4892,7 +4931,7 @@
       <c r="L119" s="42"/>
       <c r="M119" s="42"/>
     </row>
-    <row r="120" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" s="43" customFormat="1">
       <c r="A120" s="42"/>
       <c r="B120" s="42"/>
       <c r="C120" s="27" t="s">
@@ -4909,9 +4948,9 @@
       <c r="L120" s="42"/>
       <c r="M120" s="42"/>
     </row>
-    <row r="121" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" s="43" customFormat="1">
       <c r="A121" s="42"/>
-      <c r="B121" s="228"/>
+      <c r="B121" s="155"/>
       <c r="C121" s="27" t="s">
         <v>24</v>
       </c>
@@ -4926,9 +4965,9 @@
       <c r="L121" s="42"/>
       <c r="M121" s="42"/>
     </row>
-    <row r="122" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" s="43" customFormat="1">
       <c r="A122" s="42"/>
-      <c r="B122" s="228"/>
+      <c r="B122" s="155"/>
       <c r="C122" s="27" t="s">
         <v>25</v>
       </c>
@@ -4943,7 +4982,7 @@
       <c r="L122" s="42"/>
       <c r="M122" s="42"/>
     </row>
-    <row r="123" spans="1:17" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" s="51" customFormat="1" ht="18">
       <c r="A123" s="47" t="s">
         <v>78</v>
       </c>
@@ -4966,7 +5005,7 @@
       <c r="P123" s="50"/>
       <c r="Q123" s="50"/>
     </row>
-    <row r="124" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A124" s="52" t="s">
         <v>79</v>
       </c>
@@ -4991,7 +5030,7 @@
       <c r="P124" s="50"/>
       <c r="Q124" s="50"/>
     </row>
-    <row r="125" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" s="51" customFormat="1">
       <c r="A125" s="53"/>
       <c r="B125" s="53"/>
       <c r="C125" s="53" t="s">
@@ -5012,7 +5051,7 @@
       <c r="P125" s="50"/>
       <c r="Q125" s="50"/>
     </row>
-    <row r="126" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" s="51" customFormat="1">
       <c r="A126" s="53"/>
       <c r="B126" s="53"/>
       <c r="C126" s="53" t="s">
@@ -5033,7 +5072,7 @@
       <c r="P126" s="50"/>
       <c r="Q126" s="50"/>
     </row>
-    <row r="127" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" s="51" customFormat="1">
       <c r="A127" s="53"/>
       <c r="B127" s="53"/>
       <c r="C127" s="53" t="s">
@@ -5054,7 +5093,7 @@
       <c r="P127" s="50"/>
       <c r="Q127" s="50"/>
     </row>
-    <row r="128" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" s="51" customFormat="1">
       <c r="A128" s="53"/>
       <c r="B128" s="53"/>
       <c r="C128" s="53" t="s">
@@ -5075,7 +5114,7 @@
       <c r="P128" s="50"/>
       <c r="Q128" s="50"/>
     </row>
-    <row r="129" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" s="51" customFormat="1">
       <c r="A129" s="53"/>
       <c r="B129" s="53"/>
       <c r="C129" s="53" t="s">
@@ -5096,7 +5135,7 @@
       <c r="P129" s="50"/>
       <c r="Q129" s="50"/>
     </row>
-    <row r="130" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" s="51" customFormat="1">
       <c r="A130" s="53"/>
       <c r="B130" s="53"/>
       <c r="C130" s="53" t="s">
@@ -5117,7 +5156,7 @@
       <c r="P130" s="50"/>
       <c r="Q130" s="50"/>
     </row>
-    <row r="131" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" s="51" customFormat="1">
       <c r="A131" s="53"/>
       <c r="B131" s="53"/>
       <c r="C131" s="53" t="s">
@@ -5138,7 +5177,7 @@
       <c r="P131" s="50"/>
       <c r="Q131" s="50"/>
     </row>
-    <row r="132" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" s="51" customFormat="1">
       <c r="A132" s="53"/>
       <c r="B132" s="53"/>
       <c r="C132" s="53" t="s">
@@ -5159,7 +5198,7 @@
       <c r="P132" s="50"/>
       <c r="Q132" s="50"/>
     </row>
-    <row r="133" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" s="51" customFormat="1">
       <c r="A133" s="53"/>
       <c r="B133" s="53"/>
       <c r="C133" s="53" t="s">
@@ -5180,7 +5219,7 @@
       <c r="P133" s="50"/>
       <c r="Q133" s="50"/>
     </row>
-    <row r="134" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" s="51" customFormat="1">
       <c r="A134" s="53"/>
       <c r="B134" s="53"/>
       <c r="C134" s="53" t="s">
@@ -5201,7 +5240,7 @@
       <c r="P134" s="50"/>
       <c r="Q134" s="50"/>
     </row>
-    <row r="135" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" s="51" customFormat="1">
       <c r="A135" s="53"/>
       <c r="B135" s="53"/>
       <c r="C135" s="53" t="s">
@@ -5222,7 +5261,7 @@
       <c r="P135" s="50"/>
       <c r="Q135" s="50"/>
     </row>
-    <row r="136" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" s="51" customFormat="1">
       <c r="A136" s="53"/>
       <c r="B136" s="56"/>
       <c r="C136" s="53"/>
@@ -5241,7 +5280,7 @@
       <c r="P136" s="50"/>
       <c r="Q136" s="50"/>
     </row>
-    <row r="137" spans="1:17" s="51" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" s="51" customFormat="1" ht="187.25">
       <c r="A137" s="45" t="s">
         <v>130</v>
       </c>
@@ -5272,7 +5311,7 @@
       <c r="P137" s="50"/>
       <c r="Q137" s="50"/>
     </row>
-    <row r="138" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A138" s="53"/>
       <c r="B138" s="56"/>
       <c r="C138" s="53"/>
@@ -5297,7 +5336,7 @@
       <c r="P138" s="50"/>
       <c r="Q138" s="50"/>
     </row>
-    <row r="139" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" s="51" customFormat="1">
       <c r="A139" s="53"/>
       <c r="B139" s="56"/>
       <c r="C139" s="53"/>
@@ -5316,7 +5355,7 @@
       <c r="P139" s="50"/>
       <c r="Q139" s="50"/>
     </row>
-    <row r="140" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" s="51" customFormat="1">
       <c r="A140" s="53"/>
       <c r="B140" s="56"/>
       <c r="C140" s="53"/>
@@ -5335,7 +5374,7 @@
       <c r="P140" s="50"/>
       <c r="Q140" s="50"/>
     </row>
-    <row r="141" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" s="51" customFormat="1">
       <c r="A141" s="53"/>
       <c r="B141" s="56"/>
       <c r="C141" s="53"/>
@@ -5354,7 +5393,7 @@
       <c r="P141" s="50"/>
       <c r="Q141" s="50"/>
     </row>
-    <row r="142" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" s="51" customFormat="1">
       <c r="A142" s="53"/>
       <c r="B142" s="56"/>
       <c r="C142" s="53"/>
@@ -5373,11 +5412,11 @@
       <c r="P142" s="50"/>
       <c r="Q142" s="50"/>
     </row>
-    <row r="143" spans="1:17" s="51" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" s="51" customFormat="1" ht="46.75">
       <c r="A143" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B143" s="73" t="s">
+      <c r="B143" s="185" t="s">
         <v>132</v>
       </c>
       <c r="C143" s="60"/>
@@ -5406,9 +5445,9 @@
       <c r="P143" s="50"/>
       <c r="Q143" s="50"/>
     </row>
-    <row r="144" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A144" s="53"/>
-      <c r="B144" s="74"/>
+      <c r="B144" s="186"/>
       <c r="C144" s="60"/>
       <c r="D144" s="54"/>
       <c r="E144" s="55"/>
@@ -5433,9 +5472,9 @@
       <c r="P144" s="50"/>
       <c r="Q144" s="50"/>
     </row>
-    <row r="145" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A145" s="53"/>
-      <c r="B145" s="74"/>
+      <c r="B145" s="186"/>
       <c r="C145" s="60"/>
       <c r="D145" s="54"/>
       <c r="E145" s="55"/>
@@ -5460,9 +5499,9 @@
       <c r="P145" s="50"/>
       <c r="Q145" s="50"/>
     </row>
-    <row r="146" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="51" customFormat="1">
       <c r="A146" s="53"/>
-      <c r="B146" s="74"/>
+      <c r="B146" s="186"/>
       <c r="C146" s="60"/>
       <c r="D146" s="54"/>
       <c r="E146" s="55"/>
@@ -5479,9 +5518,9 @@
       <c r="P146" s="50"/>
       <c r="Q146" s="50"/>
     </row>
-    <row r="147" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" s="51" customFormat="1">
       <c r="A147" s="53"/>
-      <c r="B147" s="74"/>
+      <c r="B147" s="186"/>
       <c r="C147" s="60"/>
       <c r="D147" s="54"/>
       <c r="E147" s="55"/>
@@ -5498,9 +5537,9 @@
       <c r="P147" s="50"/>
       <c r="Q147" s="50"/>
     </row>
-    <row r="148" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" s="51" customFormat="1">
       <c r="A148" s="53"/>
-      <c r="B148" s="74"/>
+      <c r="B148" s="186"/>
       <c r="C148" s="60"/>
       <c r="D148" s="54"/>
       <c r="E148" s="55"/>
@@ -5517,9 +5556,9 @@
       <c r="P148" s="50"/>
       <c r="Q148" s="50"/>
     </row>
-    <row r="149" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" s="51" customFormat="1">
       <c r="A149" s="53"/>
-      <c r="B149" s="74"/>
+      <c r="B149" s="186"/>
       <c r="C149" s="60"/>
       <c r="D149" s="54"/>
       <c r="E149" s="55"/>
@@ -5536,9 +5575,9 @@
       <c r="P149" s="50"/>
       <c r="Q149" s="50"/>
     </row>
-    <row r="150" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" s="51" customFormat="1">
       <c r="A150" s="53"/>
-      <c r="B150" s="75"/>
+      <c r="B150" s="187"/>
       <c r="C150" s="60"/>
       <c r="D150" s="54"/>
       <c r="E150" s="55"/>
@@ -5555,11 +5594,11 @@
       <c r="P150" s="50"/>
       <c r="Q150" s="50"/>
     </row>
-    <row r="151" spans="1:17" s="51" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" s="51" customFormat="1" ht="46.75">
       <c r="A151" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B151" s="73" t="s">
+      <c r="B151" s="185" t="s">
         <v>89</v>
       </c>
       <c r="C151" s="60"/>
@@ -5588,9 +5627,9 @@
       <c r="P151" s="50"/>
       <c r="Q151" s="50"/>
     </row>
-    <row r="152" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A152" s="62"/>
-      <c r="B152" s="74"/>
+      <c r="B152" s="186"/>
       <c r="C152" s="60"/>
       <c r="D152" s="54"/>
       <c r="E152" s="55"/>
@@ -5613,9 +5652,9 @@
       <c r="P152" s="50"/>
       <c r="Q152" s="50"/>
     </row>
-    <row r="153" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A153" s="62"/>
-      <c r="B153" s="74"/>
+      <c r="B153" s="186"/>
       <c r="C153" s="60"/>
       <c r="D153" s="54"/>
       <c r="E153" s="55"/>
@@ -5638,9 +5677,9 @@
       <c r="P153" s="50"/>
       <c r="Q153" s="50"/>
     </row>
-    <row r="154" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" s="51" customFormat="1">
       <c r="A154" s="62"/>
-      <c r="B154" s="74"/>
+      <c r="B154" s="186"/>
       <c r="C154" s="60"/>
       <c r="D154" s="54"/>
       <c r="E154" s="55"/>
@@ -5657,9 +5696,9 @@
       <c r="P154" s="50"/>
       <c r="Q154" s="50"/>
     </row>
-    <row r="155" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" s="51" customFormat="1">
       <c r="A155" s="63"/>
-      <c r="B155" s="74"/>
+      <c r="B155" s="186"/>
       <c r="C155" s="60"/>
       <c r="D155" s="54"/>
       <c r="E155" s="55"/>
@@ -5676,9 +5715,9 @@
       <c r="P155" s="50"/>
       <c r="Q155" s="50"/>
     </row>
-    <row r="156" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" s="51" customFormat="1">
       <c r="A156" s="63"/>
-      <c r="B156" s="74"/>
+      <c r="B156" s="186"/>
       <c r="C156" s="60"/>
       <c r="D156" s="54"/>
       <c r="E156" s="55"/>
@@ -5695,9 +5734,9 @@
       <c r="P156" s="50"/>
       <c r="Q156" s="50"/>
     </row>
-    <row r="157" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" s="51" customFormat="1">
       <c r="A157" s="63"/>
-      <c r="B157" s="74"/>
+      <c r="B157" s="186"/>
       <c r="C157" s="60"/>
       <c r="D157" s="54"/>
       <c r="E157" s="55"/>
@@ -5714,9 +5753,9 @@
       <c r="P157" s="50"/>
       <c r="Q157" s="50"/>
     </row>
-    <row r="158" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" s="51" customFormat="1">
       <c r="A158" s="63"/>
-      <c r="B158" s="74"/>
+      <c r="B158" s="186"/>
       <c r="C158" s="60"/>
       <c r="D158" s="54"/>
       <c r="E158" s="55"/>
@@ -5733,9 +5772,9 @@
       <c r="P158" s="50"/>
       <c r="Q158" s="50"/>
     </row>
-    <row r="159" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" s="51" customFormat="1">
       <c r="A159" s="63"/>
-      <c r="B159" s="75"/>
+      <c r="B159" s="187"/>
       <c r="C159" s="60"/>
       <c r="D159" s="54"/>
       <c r="E159" s="55"/>
@@ -5752,11 +5791,11 @@
       <c r="P159" s="50"/>
       <c r="Q159" s="50"/>
     </row>
-    <row r="160" spans="1:17" s="51" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" s="51" customFormat="1" ht="46.75">
       <c r="A160" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="B160" s="73" t="s">
+      <c r="B160" s="185" t="s">
         <v>92</v>
       </c>
       <c r="C160" s="60"/>
@@ -5781,9 +5820,9 @@
       <c r="P160" s="50"/>
       <c r="Q160" s="50"/>
     </row>
-    <row r="161" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A161" s="62"/>
-      <c r="B161" s="74"/>
+      <c r="B161" s="186"/>
       <c r="C161" s="60"/>
       <c r="D161" s="54"/>
       <c r="E161" s="55"/>
@@ -5806,9 +5845,9 @@
       <c r="P161" s="50"/>
       <c r="Q161" s="50"/>
     </row>
-    <row r="162" spans="1:17" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" s="51" customFormat="1" ht="31.25">
       <c r="A162" s="62"/>
-      <c r="B162" s="74"/>
+      <c r="B162" s="186"/>
       <c r="C162" s="60"/>
       <c r="D162" s="54"/>
       <c r="E162" s="55"/>
@@ -5829,9 +5868,9 @@
       <c r="P162" s="50"/>
       <c r="Q162" s="50"/>
     </row>
-    <row r="163" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" s="51" customFormat="1">
       <c r="A163" s="62"/>
-      <c r="B163" s="74"/>
+      <c r="B163" s="186"/>
       <c r="C163" s="60"/>
       <c r="D163" s="54"/>
       <c r="E163" s="55"/>
@@ -5848,9 +5887,9 @@
       <c r="P163" s="50"/>
       <c r="Q163" s="50"/>
     </row>
-    <row r="164" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" s="51" customFormat="1">
       <c r="A164" s="63"/>
-      <c r="B164" s="74"/>
+      <c r="B164" s="186"/>
       <c r="C164" s="60"/>
       <c r="D164" s="54"/>
       <c r="E164" s="55"/>
@@ -5867,9 +5906,9 @@
       <c r="P164" s="50"/>
       <c r="Q164" s="50"/>
     </row>
-    <row r="165" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" s="51" customFormat="1">
       <c r="A165" s="63"/>
-      <c r="B165" s="74"/>
+      <c r="B165" s="186"/>
       <c r="C165" s="60"/>
       <c r="D165" s="54"/>
       <c r="E165" s="55"/>
@@ -5886,9 +5925,9 @@
       <c r="P165" s="50"/>
       <c r="Q165" s="50"/>
     </row>
-    <row r="166" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" s="51" customFormat="1">
       <c r="A166" s="63"/>
-      <c r="B166" s="74"/>
+      <c r="B166" s="186"/>
       <c r="C166" s="60"/>
       <c r="D166" s="54"/>
       <c r="E166" s="55"/>
@@ -5905,9 +5944,9 @@
       <c r="P166" s="50"/>
       <c r="Q166" s="50"/>
     </row>
-    <row r="167" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" s="51" customFormat="1">
       <c r="A167" s="63"/>
-      <c r="B167" s="74"/>
+      <c r="B167" s="186"/>
       <c r="C167" s="60"/>
       <c r="D167" s="54"/>
       <c r="E167" s="55"/>
@@ -5924,9 +5963,9 @@
       <c r="P167" s="50"/>
       <c r="Q167" s="50"/>
     </row>
-    <row r="168" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" s="51" customFormat="1">
       <c r="A168" s="63"/>
-      <c r="B168" s="74"/>
+      <c r="B168" s="186"/>
       <c r="C168" s="60"/>
       <c r="D168" s="54"/>
       <c r="E168" s="55"/>
@@ -5943,9 +5982,9 @@
       <c r="P168" s="50"/>
       <c r="Q168" s="50"/>
     </row>
-    <row r="169" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" s="51" customFormat="1">
       <c r="A169" s="63"/>
-      <c r="B169" s="74"/>
+      <c r="B169" s="186"/>
       <c r="C169" s="60"/>
       <c r="D169" s="54"/>
       <c r="E169" s="55"/>
@@ -5962,9 +6001,9 @@
       <c r="P169" s="50"/>
       <c r="Q169" s="50"/>
     </row>
-    <row r="170" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" s="51" customFormat="1">
       <c r="A170" s="63"/>
-      <c r="B170" s="74"/>
+      <c r="B170" s="186"/>
       <c r="C170" s="60"/>
       <c r="D170" s="54"/>
       <c r="E170" s="55"/>
@@ -5981,9 +6020,9 @@
       <c r="P170" s="50"/>
       <c r="Q170" s="50"/>
     </row>
-    <row r="171" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" s="51" customFormat="1">
       <c r="A171" s="63"/>
-      <c r="B171" s="75"/>
+      <c r="B171" s="187"/>
       <c r="C171" s="60"/>
       <c r="D171" s="54"/>
       <c r="E171" s="55"/>
@@ -6000,7 +6039,7 @@
       <c r="P171" s="50"/>
       <c r="Q171" s="50"/>
     </row>
-    <row r="172" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" s="51" customFormat="1">
       <c r="A172" s="55"/>
       <c r="B172" s="55"/>
       <c r="C172" s="55"/>
@@ -6019,7 +6058,7 @@
       <c r="P172" s="50"/>
       <c r="Q172" s="50"/>
     </row>
-    <row r="173" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" s="51" customFormat="1">
       <c r="A173" s="55"/>
       <c r="B173" s="55"/>
       <c r="C173" s="55"/>
@@ -6038,7 +6077,7 @@
       <c r="P173" s="50"/>
       <c r="Q173" s="50"/>
     </row>
-    <row r="174" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" s="51" customFormat="1">
       <c r="A174" s="55"/>
       <c r="B174" s="55"/>
       <c r="C174" s="55"/>
@@ -6057,7 +6096,7 @@
       <c r="P174" s="50"/>
       <c r="Q174" s="50"/>
     </row>
-    <row r="175" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" s="51" customFormat="1">
       <c r="A175" s="55"/>
       <c r="B175" s="55"/>
       <c r="C175" s="55"/>
@@ -6076,13 +6115,13 @@
       <c r="P175" s="50"/>
       <c r="Q175" s="50"/>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17">
       <c r="N176" s="38"/>
       <c r="O176" s="38"/>
       <c r="P176" s="38"/>
       <c r="Q176" s="38"/>
     </row>
-    <row r="177" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="14:17">
       <c r="N177" s="37"/>
       <c r="O177" s="37"/>
       <c r="P177" s="37"/>
@@ -6090,16 +6129,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="I76:I78"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="I100:I102"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="B63:B74"/>
+    <mergeCell ref="B54:B62"/>
+    <mergeCell ref="B21:B32"/>
+    <mergeCell ref="B34:B45"/>
     <mergeCell ref="B143:B150"/>
     <mergeCell ref="B151:B159"/>
     <mergeCell ref="B160:B171"/>
@@ -6108,12 +6143,16 @@
     <mergeCell ref="A75:A77"/>
     <mergeCell ref="B75:B79"/>
     <mergeCell ref="B111:B113"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B46:B53"/>
-    <mergeCell ref="B63:B74"/>
-    <mergeCell ref="B54:B62"/>
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="B34:B45"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="I100:I102"/>
+    <mergeCell ref="I112:I114"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="I115:I117"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="I76:I78"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
@@ -6146,7 +6185,7 @@
     <hyperlink ref="M111" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId29"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6159,805 +6198,813 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="29.09765625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="27.296875" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" style="51" customWidth="1"/>
-    <col min="6" max="6" width="18.09765625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="18.69921875" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.8984375" style="51"/>
+    <col min="1" max="1" width="15.625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="29.125" style="51" customWidth="1"/>
+    <col min="3" max="3" width="27.25" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="51" customWidth="1"/>
+    <col min="6" max="6" width="18.125" style="51" customWidth="1"/>
+    <col min="7" max="7" width="18.75" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="51"/>
     <col min="9" max="9" width="12" style="51" customWidth="1"/>
-    <col min="10" max="10" width="12.19921875" style="51" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" style="51" customWidth="1"/>
-    <col min="12" max="12" width="12.19921875" style="51" customWidth="1"/>
-    <col min="13" max="13" width="13.3984375" style="51" customWidth="1"/>
-    <col min="14" max="16" width="8.8984375" style="51"/>
-    <col min="17" max="17" width="9.3984375" style="51" customWidth="1"/>
-    <col min="18" max="16384" width="8.8984375" style="51"/>
+    <col min="10" max="10" width="12.25" style="51" customWidth="1"/>
+    <col min="11" max="11" width="10.625" style="51" customWidth="1"/>
+    <col min="12" max="12" width="12.25" style="51" customWidth="1"/>
+    <col min="13" max="13" width="13.375" style="51" customWidth="1"/>
+    <col min="14" max="16" width="8.875" style="51"/>
+    <col min="17" max="17" width="9.375" style="51" customWidth="1"/>
+    <col min="18" max="16384" width="8.875" style="51"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="80" t="s">
+    <row r="4" spans="1:17" ht="16.25" thickBot="1">
+      <c r="E4" s="67" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+    <row r="5" spans="1:17" ht="16.25" thickBot="1">
+      <c r="A5" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="83" t="s">
+      <c r="B5" s="69"/>
+      <c r="C5" s="204" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="85" t="s">
+      <c r="D5" s="204"/>
+      <c r="E5" s="204"/>
+      <c r="F5" s="204"/>
+      <c r="G5" s="204"/>
+      <c r="H5" s="204"/>
+      <c r="I5" s="204"/>
+      <c r="J5" s="204"/>
+      <c r="K5" s="204"/>
+      <c r="L5" s="204"/>
+      <c r="M5" s="205"/>
+      <c r="N5" s="206" t="s">
         <v>97</v>
       </c>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-    </row>
-    <row r="6" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="O5" s="207"/>
+      <c r="P5" s="207"/>
+      <c r="Q5" s="207"/>
+    </row>
+    <row r="6" spans="1:17" ht="24" customHeight="1">
+      <c r="A6" s="208" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="231" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="89" t="s">
+      <c r="C6" s="220" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="89"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91" t="s">
+      <c r="D6" s="220"/>
+      <c r="E6" s="221"/>
+      <c r="F6" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="G6" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="218" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="93" t="s">
+      <c r="I6" s="210" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="94"/>
-      <c r="K6" s="95" t="s">
+      <c r="J6" s="211"/>
+      <c r="K6" s="216" t="s">
         <v>108</v>
       </c>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="97" t="s">
+      <c r="M6" s="214" t="s">
         <v>110</v>
       </c>
-      <c r="N6" s="98" t="s">
+      <c r="N6" s="229" t="s">
         <v>100</v>
       </c>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="225" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="99" t="s">
+      <c r="P6" s="225" t="s">
         <v>102</v>
       </c>
-      <c r="Q6" s="100" t="s">
+      <c r="Q6" s="227" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="103" t="s">
+    <row r="7" spans="1:17" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A7" s="209"/>
+      <c r="B7" s="232"/>
+      <c r="C7" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="I7" s="106" t="s">
+      <c r="H7" s="219"/>
+      <c r="I7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="108" t="s">
+      <c r="J7" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="113"/>
-      <c r="Q7" s="114"/>
-    </row>
-    <row r="8" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="115" t="s">
+      <c r="K7" s="217"/>
+      <c r="L7" s="213"/>
+      <c r="M7" s="215"/>
+      <c r="N7" s="230"/>
+      <c r="O7" s="226"/>
+      <c r="P7" s="226"/>
+      <c r="Q7" s="228"/>
+    </row>
+    <row r="8" spans="1:17" ht="22.5" customHeight="1">
+      <c r="A8" s="223" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="117"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="119">
+      <c r="C8" s="77"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="79">
         <v>6</v>
       </c>
-      <c r="F8" s="119">
+      <c r="F8" s="79">
         <v>2</v>
       </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119">
+      <c r="G8" s="79"/>
+      <c r="H8" s="79">
         <v>4</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="120">
+      <c r="I8" s="79"/>
+      <c r="J8" s="80">
         <v>12</v>
       </c>
-      <c r="K8" s="121">
+      <c r="K8" s="81">
         <v>3</v>
       </c>
-      <c r="L8" s="118"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="123" t="s">
+      <c r="L8" s="78"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="122"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
-      <c r="B9" s="125" t="s">
+      <c r="O8" s="84"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="82"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="223"/>
+      <c r="B9" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="126">
+      <c r="C9" s="86">
         <v>1</v>
       </c>
-      <c r="D9" s="127">
+      <c r="D9" s="87">
         <v>5</v>
       </c>
-      <c r="E9" s="127">
+      <c r="E9" s="87">
         <v>4</v>
       </c>
-      <c r="F9" s="128">
+      <c r="F9" s="88">
         <v>2</v>
       </c>
-      <c r="G9" s="128"/>
-      <c r="H9" s="119">
+      <c r="G9" s="88"/>
+      <c r="H9" s="79">
         <v>4</v>
       </c>
-      <c r="I9" s="127"/>
-      <c r="J9" s="129">
+      <c r="I9" s="87"/>
+      <c r="J9" s="89">
         <v>12</v>
       </c>
-      <c r="K9" s="130">
+      <c r="K9" s="90">
         <v>2</v>
       </c>
-      <c r="L9" s="127"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="123" t="s">
+      <c r="L9" s="87"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-      <c r="Q9" s="132"/>
-    </row>
-    <row r="10" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134" t="s">
+      <c r="O9" s="84"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="92"/>
+    </row>
+    <row r="10" spans="1:17" ht="21" customHeight="1">
+      <c r="A10" s="224"/>
+      <c r="B10" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="135">
+      <c r="C10" s="94">
         <v>1</v>
       </c>
-      <c r="D10" s="136">
+      <c r="D10" s="95">
         <v>6</v>
       </c>
-      <c r="E10" s="136">
+      <c r="E10" s="95">
         <v>1</v>
       </c>
-      <c r="F10" s="137">
+      <c r="F10" s="96">
         <v>2</v>
       </c>
-      <c r="G10" s="137"/>
-      <c r="H10" s="119">
+      <c r="G10" s="96"/>
+      <c r="H10" s="79">
         <v>4</v>
       </c>
-      <c r="I10" s="136"/>
-      <c r="J10" s="138">
+      <c r="I10" s="95"/>
+      <c r="J10" s="97">
         <v>12</v>
       </c>
-      <c r="K10" s="139">
+      <c r="K10" s="98">
         <v>2</v>
       </c>
-      <c r="L10" s="136">
+      <c r="L10" s="95">
         <v>1</v>
       </c>
-      <c r="M10" s="140"/>
-      <c r="N10" s="141" t="s">
+      <c r="M10" s="99"/>
+      <c r="N10" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="143"/>
-    </row>
-    <row r="11" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="144" t="s">
+      <c r="O10" s="101"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="102"/>
+    </row>
+    <row r="11" spans="1:17" ht="43.25">
+      <c r="A11" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="145" t="s">
+      <c r="B11" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="146" t="s">
+      <c r="C11" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="147"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148">
+      <c r="D11" s="106"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107">
         <v>2</v>
       </c>
-      <c r="G11" s="148"/>
-      <c r="H11" s="119">
+      <c r="G11" s="107"/>
+      <c r="H11" s="79">
         <v>4</v>
       </c>
-      <c r="I11" s="148"/>
-      <c r="J11" s="149">
+      <c r="I11" s="107"/>
+      <c r="J11" s="108">
         <v>12</v>
       </c>
-      <c r="K11" s="150">
+      <c r="K11" s="109">
         <v>3</v>
       </c>
-      <c r="L11" s="148"/>
-      <c r="M11" s="151"/>
-      <c r="N11" s="152" t="s">
+      <c r="L11" s="107"/>
+      <c r="M11" s="110"/>
+      <c r="N11" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="153"/>
-      <c r="P11" s="153"/>
-      <c r="Q11" s="154"/>
-    </row>
-    <row r="12" spans="1:17" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="155" t="s">
+      <c r="O11" s="112"/>
+      <c r="P11" s="112"/>
+      <c r="Q11" s="113"/>
+    </row>
+    <row r="12" spans="1:17" ht="63" customHeight="1">
+      <c r="A12" s="114" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="145" t="s">
+      <c r="B12" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="146">
+      <c r="C12" s="105">
         <v>0</v>
       </c>
-      <c r="D12" s="146"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148">
+      <c r="D12" s="105"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107">
         <v>2</v>
       </c>
-      <c r="G12" s="148"/>
-      <c r="H12" s="119">
+      <c r="G12" s="107"/>
+      <c r="H12" s="79">
         <v>4</v>
       </c>
-      <c r="I12" s="148"/>
-      <c r="J12" s="149">
+      <c r="I12" s="107"/>
+      <c r="J12" s="108">
         <v>12</v>
       </c>
-      <c r="K12" s="150"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="151"/>
-      <c r="N12" s="152" t="s">
+      <c r="K12" s="109"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="110"/>
+      <c r="N12" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="153"/>
-      <c r="P12" s="153"/>
-      <c r="Q12" s="154"/>
-    </row>
-    <row r="13" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="156" t="s">
+      <c r="O12" s="112"/>
+      <c r="P12" s="112"/>
+      <c r="Q12" s="113"/>
+    </row>
+    <row r="13" spans="1:17" ht="29.5" thickBot="1">
+      <c r="A13" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="158" t="s">
+      <c r="C13" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="159"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159">
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118">
         <v>2</v>
       </c>
-      <c r="G13" s="159"/>
-      <c r="H13" s="229">
+      <c r="G13" s="118"/>
+      <c r="H13" s="156">
         <v>4</v>
       </c>
-      <c r="I13" s="159"/>
-      <c r="J13" s="160">
+      <c r="I13" s="118"/>
+      <c r="J13" s="119">
         <v>12</v>
       </c>
-      <c r="K13" s="161">
+      <c r="K13" s="120">
         <v>3</v>
       </c>
-      <c r="L13" s="159"/>
-      <c r="M13" s="162"/>
-      <c r="N13" s="163" t="s">
+      <c r="L13" s="118"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="164"/>
-      <c r="P13" s="165"/>
-      <c r="Q13" s="166"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="167"/>
-    </row>
-    <row r="15" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="168" t="s">
+      <c r="O13" s="123"/>
+      <c r="P13" s="124"/>
+      <c r="Q13" s="125"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="126"/>
+    </row>
+    <row r="15" spans="1:17" ht="16.25" thickBot="1"/>
+    <row r="16" spans="1:17" ht="16.25" thickBot="1">
+      <c r="A16" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="169"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="170" t="s">
+      <c r="B16" s="128"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="222" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="129" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="175"/>
-      <c r="D17" s="172"/>
-      <c r="E17" s="173">
+      <c r="C17" s="133"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="131">
         <v>6</v>
       </c>
-      <c r="F17" s="173">
+      <c r="F17" s="131">
         <v>2</v>
       </c>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173">
+      <c r="G17" s="131"/>
+      <c r="H17" s="131">
         <v>4</v>
       </c>
-      <c r="I17" s="173"/>
-      <c r="J17" s="174">
+      <c r="I17" s="131"/>
+      <c r="J17" s="132">
         <v>12</v>
       </c>
-      <c r="K17" s="175">
+      <c r="K17" s="133">
         <v>3</v>
       </c>
-      <c r="L17" s="172"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="177"/>
-      <c r="O17" s="178" t="s">
+      <c r="L17" s="130"/>
+      <c r="M17" s="134"/>
+      <c r="N17" s="135"/>
+      <c r="O17" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="P17" s="178"/>
-      <c r="Q17" s="176"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
-      <c r="B18" s="125" t="s">
+      <c r="P17" s="136"/>
+      <c r="Q17" s="134"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="223"/>
+      <c r="B18" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="230">
+      <c r="C18" s="157">
         <v>1</v>
       </c>
-      <c r="D18" s="127">
+      <c r="D18" s="87">
         <v>5</v>
       </c>
-      <c r="E18" s="127">
+      <c r="E18" s="87">
         <v>4</v>
       </c>
-      <c r="F18" s="128">
+      <c r="F18" s="88">
         <v>2</v>
       </c>
-      <c r="G18" s="128"/>
-      <c r="H18" s="119">
+      <c r="G18" s="88"/>
+      <c r="H18" s="79">
         <v>4</v>
       </c>
-      <c r="I18" s="127"/>
-      <c r="J18" s="129">
+      <c r="I18" s="87"/>
+      <c r="J18" s="89">
         <v>12</v>
       </c>
-      <c r="K18" s="130">
+      <c r="K18" s="90">
         <v>2</v>
       </c>
-      <c r="L18" s="127"/>
-      <c r="M18" s="131"/>
-      <c r="N18" s="123"/>
-      <c r="O18" s="124" t="s">
+      <c r="L18" s="87"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="132"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="133"/>
-      <c r="B19" s="134" t="s">
+      <c r="P18" s="84"/>
+      <c r="Q18" s="92"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="224"/>
+      <c r="B19" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="231">
+      <c r="C19" s="158">
         <v>1</v>
       </c>
-      <c r="D19" s="136">
+      <c r="D19" s="95">
         <v>6</v>
       </c>
-      <c r="E19" s="136">
+      <c r="E19" s="95">
         <v>1</v>
       </c>
-      <c r="F19" s="137">
+      <c r="F19" s="96">
         <v>2</v>
       </c>
-      <c r="G19" s="137"/>
-      <c r="H19" s="119">
+      <c r="G19" s="96"/>
+      <c r="H19" s="79">
         <v>4</v>
       </c>
-      <c r="I19" s="136"/>
-      <c r="J19" s="138">
+      <c r="I19" s="95"/>
+      <c r="J19" s="97">
         <v>12</v>
       </c>
-      <c r="K19" s="139">
+      <c r="K19" s="98">
         <v>2</v>
       </c>
-      <c r="L19" s="136">
+      <c r="L19" s="95">
         <v>1</v>
       </c>
-      <c r="M19" s="140"/>
-      <c r="N19" s="141"/>
-      <c r="O19" s="142" t="s">
+      <c r="M19" s="99"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="P19" s="142"/>
-      <c r="Q19" s="143"/>
-    </row>
-    <row r="20" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="144" t="s">
+      <c r="P19" s="101"/>
+      <c r="Q19" s="102"/>
+    </row>
+    <row r="20" spans="1:17" ht="43.25">
+      <c r="A20" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="145" t="s">
+      <c r="B20" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="150" t="s">
+      <c r="C20" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="147"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148">
+      <c r="D20" s="106"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107">
         <v>2</v>
       </c>
-      <c r="G20" s="148"/>
-      <c r="H20" s="119">
+      <c r="G20" s="107"/>
+      <c r="H20" s="79">
         <v>4</v>
       </c>
-      <c r="I20" s="148"/>
-      <c r="J20" s="149">
+      <c r="I20" s="107"/>
+      <c r="J20" s="108">
         <v>12</v>
       </c>
-      <c r="K20" s="150">
+      <c r="K20" s="109">
         <v>3</v>
       </c>
-      <c r="L20" s="148"/>
-      <c r="M20" s="151"/>
-      <c r="N20" s="152"/>
-      <c r="O20" s="153" t="s">
+      <c r="L20" s="107"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="111"/>
+      <c r="O20" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="153"/>
-      <c r="Q20" s="154"/>
-    </row>
-    <row r="21" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="155" t="s">
+      <c r="P20" s="112"/>
+      <c r="Q20" s="113"/>
+    </row>
+    <row r="21" spans="1:17" ht="57.5">
+      <c r="A21" s="114" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="150">
+      <c r="C21" s="109">
         <v>0</v>
       </c>
-      <c r="D21" s="146"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148">
+      <c r="D21" s="105"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107">
         <v>2</v>
       </c>
-      <c r="G21" s="148"/>
-      <c r="H21" s="119">
+      <c r="G21" s="107"/>
+      <c r="H21" s="79">
         <v>4</v>
       </c>
-      <c r="I21" s="148"/>
-      <c r="J21" s="149">
+      <c r="I21" s="107"/>
+      <c r="J21" s="108">
         <v>12</v>
       </c>
-      <c r="K21" s="150"/>
-      <c r="L21" s="148"/>
-      <c r="M21" s="151"/>
-      <c r="N21" s="152"/>
-      <c r="O21" s="153" t="s">
+      <c r="K21" s="109"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="P21" s="153"/>
-      <c r="Q21" s="154"/>
-    </row>
-    <row r="22" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="156" t="s">
+      <c r="P21" s="112"/>
+      <c r="Q21" s="113"/>
+    </row>
+    <row r="22" spans="1:17" ht="29.5" thickBot="1">
+      <c r="A22" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="157" t="s">
+      <c r="B22" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="161" t="s">
+      <c r="C22" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="159"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159">
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118">
         <v>2</v>
       </c>
-      <c r="G22" s="159"/>
-      <c r="H22" s="232">
+      <c r="G22" s="118"/>
+      <c r="H22" s="159">
         <v>4</v>
       </c>
-      <c r="I22" s="159"/>
-      <c r="J22" s="160">
+      <c r="I22" s="118"/>
+      <c r="J22" s="119">
         <v>12</v>
       </c>
-      <c r="K22" s="161">
+      <c r="K22" s="120">
         <v>3</v>
       </c>
-      <c r="L22" s="159"/>
-      <c r="M22" s="162"/>
-      <c r="N22" s="163"/>
-      <c r="O22" s="164" t="s">
+      <c r="L22" s="118"/>
+      <c r="M22" s="121"/>
+      <c r="N22" s="122"/>
+      <c r="O22" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="P22" s="165"/>
-      <c r="Q22" s="166"/>
-    </row>
-    <row r="24" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="168" t="s">
+      <c r="P22" s="124"/>
+      <c r="Q22" s="125"/>
+    </row>
+    <row r="24" spans="1:17" ht="16.25" thickBot="1"/>
+    <row r="25" spans="1:17" ht="16.25" thickBot="1">
+      <c r="A25" s="127" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="170" t="s">
+    <row r="26" spans="1:17">
+      <c r="A26" s="222" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="171" t="s">
+      <c r="B26" s="129" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="175"/>
-      <c r="D26" s="172"/>
-      <c r="E26" s="173">
+      <c r="C26" s="133"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="131">
         <v>6</v>
       </c>
-      <c r="F26" s="173">
+      <c r="F26" s="131">
         <v>2</v>
       </c>
-      <c r="G26" s="173"/>
-      <c r="H26" s="173">
+      <c r="G26" s="131"/>
+      <c r="H26" s="131">
         <v>4</v>
       </c>
-      <c r="I26" s="173"/>
-      <c r="J26" s="174">
+      <c r="I26" s="131"/>
+      <c r="J26" s="132">
         <v>12</v>
       </c>
-      <c r="K26" s="175">
+      <c r="K26" s="133">
         <v>3</v>
       </c>
-      <c r="L26" s="172"/>
-      <c r="M26" s="176"/>
-      <c r="N26" s="177"/>
-      <c r="O26" s="178"/>
-      <c r="P26" s="178" t="s">
+      <c r="L26" s="130"/>
+      <c r="M26" s="134"/>
+      <c r="N26" s="135"/>
+      <c r="O26" s="136"/>
+      <c r="P26" s="136" t="s">
         <v>95</v>
       </c>
-      <c r="Q26" s="176"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="115"/>
-      <c r="B27" s="125" t="s">
+      <c r="Q26" s="134"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="223"/>
+      <c r="B27" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="230">
+      <c r="C27" s="157">
         <v>1</v>
       </c>
-      <c r="D27" s="127">
+      <c r="D27" s="87">
         <v>5</v>
       </c>
-      <c r="E27" s="127">
+      <c r="E27" s="87">
         <v>4</v>
       </c>
-      <c r="F27" s="128">
+      <c r="F27" s="88">
         <v>2</v>
       </c>
-      <c r="G27" s="128"/>
-      <c r="H27" s="119">
+      <c r="G27" s="88"/>
+      <c r="H27" s="79">
         <v>4</v>
       </c>
-      <c r="I27" s="127"/>
-      <c r="J27" s="129">
+      <c r="I27" s="87"/>
+      <c r="J27" s="89">
         <v>12</v>
       </c>
-      <c r="K27" s="130">
+      <c r="K27" s="90">
         <v>2</v>
       </c>
-      <c r="L27" s="127"/>
-      <c r="M27" s="131"/>
-      <c r="N27" s="123"/>
-      <c r="O27" s="124"/>
-      <c r="P27" s="124" t="s">
+      <c r="L27" s="87"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="Q27" s="132"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="133"/>
-      <c r="B28" s="134" t="s">
+      <c r="Q27" s="92"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="224"/>
+      <c r="B28" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="231">
+      <c r="C28" s="158">
         <v>1</v>
       </c>
-      <c r="D28" s="136">
+      <c r="D28" s="95">
         <v>6</v>
       </c>
-      <c r="E28" s="136">
+      <c r="E28" s="95">
         <v>1</v>
       </c>
-      <c r="F28" s="137">
+      <c r="F28" s="96">
         <v>2</v>
       </c>
-      <c r="G28" s="137"/>
-      <c r="H28" s="119">
+      <c r="G28" s="96"/>
+      <c r="H28" s="79">
         <v>4</v>
       </c>
-      <c r="I28" s="136"/>
-      <c r="J28" s="138">
+      <c r="I28" s="95"/>
+      <c r="J28" s="97">
         <v>12</v>
       </c>
-      <c r="K28" s="139">
+      <c r="K28" s="98">
         <v>2</v>
       </c>
-      <c r="L28" s="136">
+      <c r="L28" s="95">
         <v>1</v>
       </c>
-      <c r="M28" s="140"/>
-      <c r="N28" s="141"/>
-      <c r="O28" s="142"/>
-      <c r="P28" s="142" t="s">
+      <c r="M28" s="99"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="101"/>
+      <c r="P28" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="Q28" s="143"/>
-    </row>
-    <row r="29" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="144" t="s">
+      <c r="Q28" s="102"/>
+    </row>
+    <row r="29" spans="1:17" ht="43.25">
+      <c r="A29" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="145" t="s">
+      <c r="B29" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="150" t="s">
+      <c r="C29" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="147"/>
-      <c r="E29" s="148"/>
-      <c r="F29" s="148">
+      <c r="D29" s="106"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="107">
         <v>2</v>
       </c>
-      <c r="G29" s="148"/>
-      <c r="H29" s="119">
+      <c r="G29" s="107"/>
+      <c r="H29" s="79">
         <v>4</v>
       </c>
-      <c r="I29" s="148"/>
-      <c r="J29" s="149">
+      <c r="I29" s="107"/>
+      <c r="J29" s="108">
         <v>12</v>
       </c>
-      <c r="K29" s="150">
+      <c r="K29" s="109">
         <v>3</v>
       </c>
-      <c r="L29" s="148"/>
-      <c r="M29" s="151"/>
-      <c r="N29" s="152"/>
-      <c r="O29" s="153"/>
-      <c r="P29" s="153" t="s">
+      <c r="L29" s="107"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="111"/>
+      <c r="O29" s="112"/>
+      <c r="P29" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="Q29" s="154"/>
-    </row>
-    <row r="30" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="155" t="s">
+      <c r="Q29" s="113"/>
+    </row>
+    <row r="30" spans="1:17" ht="57.5">
+      <c r="A30" s="114" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="150">
+      <c r="C30" s="109">
         <v>0</v>
       </c>
-      <c r="D30" s="148"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="148">
+      <c r="D30" s="107"/>
+      <c r="E30" s="107"/>
+      <c r="F30" s="107">
         <v>2</v>
       </c>
-      <c r="G30" s="148"/>
-      <c r="H30" s="119">
+      <c r="G30" s="107"/>
+      <c r="H30" s="79">
         <v>4</v>
       </c>
-      <c r="I30" s="148"/>
-      <c r="J30" s="149">
+      <c r="I30" s="107"/>
+      <c r="J30" s="108">
         <v>12</v>
       </c>
-      <c r="K30" s="150"/>
-      <c r="L30" s="148"/>
-      <c r="M30" s="151"/>
-      <c r="N30" s="152"/>
-      <c r="O30" s="153"/>
-      <c r="P30" s="153" t="s">
+      <c r="K30" s="109"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="111"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="Q30" s="154"/>
-    </row>
-    <row r="31" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="156" t="s">
+      <c r="Q30" s="113"/>
+    </row>
+    <row r="31" spans="1:17" ht="29.5" thickBot="1">
+      <c r="A31" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="157" t="s">
+      <c r="B31" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="161" t="s">
+      <c r="C31" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="159"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="159">
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118">
         <v>2</v>
       </c>
-      <c r="G31" s="159"/>
-      <c r="H31" s="232">
+      <c r="G31" s="118"/>
+      <c r="H31" s="159">
         <v>4</v>
       </c>
-      <c r="I31" s="159"/>
-      <c r="J31" s="160">
+      <c r="I31" s="118"/>
+      <c r="J31" s="119">
         <v>12</v>
       </c>
-      <c r="K31" s="161">
+      <c r="K31" s="120">
         <v>3</v>
       </c>
-      <c r="L31" s="159"/>
-      <c r="M31" s="162"/>
-      <c r="N31" s="163"/>
-      <c r="O31" s="164"/>
-      <c r="P31" s="165" t="s">
+      <c r="L31" s="118"/>
+      <c r="M31" s="121"/>
+      <c r="N31" s="122"/>
+      <c r="O31" s="123"/>
+      <c r="P31" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="Q31" s="166"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="Q31" s="125"/>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" s="51" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="C5:M5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="A6:A7"/>
@@ -6967,16 +7014,13 @@
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>